<commit_message>
Renamed control, reduced to single
</commit_message>
<xml_diff>
--- a/summaries/representativeSampleSummary_95.xlsx
+++ b/summaries/representativeSampleSummary_95.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="206">
   <si>
     <t xml:space="preserve">Subject</t>
   </si>
@@ -617,13 +617,10 @@
     <t xml:space="preserve">307 NP-OP 20200717</t>
   </si>
   <si>
-    <t xml:space="preserve">CCLB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP0001-1m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vero cells</t>
+    <t xml:space="preserve">USA-WA1-2020-TCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP0002</t>
   </si>
   <si>
     <t xml:space="preserve">2020-03-28</t>
@@ -632,16 +629,7 @@
     <t xml:space="preserve">20200328</t>
   </si>
   <si>
-    <t xml:space="preserve">CCLB Vero cells 20200328</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP0002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E6 Vero cells 20200328</t>
+    <t xml:space="preserve">USA-WA1-2020-TCE NP-OP 20200328</t>
   </si>
 </sst>
 </file>
@@ -2799,62 +2787,29 @@
         <v>202</v>
       </c>
       <c r="C55" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D55"/>
       <c r="E55" t="s">
+        <v>72</v>
+      </c>
+      <c r="F55" t="s">
         <v>203</v>
       </c>
-      <c r="F55" t="s">
+      <c r="G55" t="n">
+        <v>30.02</v>
+      </c>
+      <c r="H55" t="n">
+        <v>99.8</v>
+      </c>
+      <c r="I55" t="n">
+        <v>99.8</v>
+      </c>
+      <c r="J55" t="s">
         <v>204</v>
       </c>
-      <c r="G55" t="n">
-        <v>27.21</v>
-      </c>
-      <c r="H55" t="n">
-        <v>99.9</v>
-      </c>
-      <c r="I55" t="n">
-        <v>99.8</v>
-      </c>
-      <c r="J55" t="s">
+      <c r="K55" t="s">
         <v>205</v>
-      </c>
-      <c r="K55" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="s">
-        <v>207</v>
-      </c>
-      <c r="B56" t="s">
-        <v>208</v>
-      </c>
-      <c r="C56" t="s">
-        <v>20</v>
-      </c>
-      <c r="D56"/>
-      <c r="E56" t="s">
-        <v>203</v>
-      </c>
-      <c r="F56" t="s">
-        <v>204</v>
-      </c>
-      <c r="G56" t="n">
-        <v>30.02</v>
-      </c>
-      <c r="H56" t="n">
-        <v>99.8</v>
-      </c>
-      <c r="I56" t="n">
-        <v>99.8</v>
-      </c>
-      <c r="J56" t="s">
-        <v>205</v>
-      </c>
-      <c r="K56" t="s">
-        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>